<commit_message>
Implement Flutter event detail screen redesign
Add responsive layout helpers and attendee avatar preview to the event
detail screen to match the new design specifications.

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/TEST-SCENARIOS.xlsx
+++ b/docs/TEST-SCENARIOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meetwithfriends\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{46C6E32E-7398-4471-9370-CA39B372D78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA33429-A68F-43BF-BB40-CC6FD3DBAD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8C4B8439-3C7D-4BF3-9C30-18CFD3954126}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="54">
   <si>
     <t>Category</t>
   </si>
@@ -175,6 +175,18 @@
   </si>
   <si>
     <t>User types invalid credentials</t>
+  </si>
+  <si>
+    <t>aandreou25</t>
+  </si>
+  <si>
+    <t>brookfieldcomfort</t>
+  </si>
+  <si>
+    <t>noodev8</t>
+  </si>
+  <si>
+    <t>Host assigns another host</t>
   </si>
 </sst>
 </file>
@@ -1042,20 +1054,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20932B91-48DE-46D3-9489-6C50CBF35969}">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.21875" customWidth="1"/>
     <col min="2" max="2" width="42.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1080,28 +1092,25 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>47</v>
@@ -1118,7 +1127,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>47</v>
@@ -1135,7 +1144,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>47</v>
@@ -1152,7 +1161,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>47</v>
@@ -1169,7 +1178,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>47</v>
@@ -1186,29 +1195,32 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1217,7 +1229,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1225,7 +1246,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1233,7 +1263,16 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1241,7 +1280,16 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1249,7 +1297,16 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1257,111 +1314,138 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>10</v>
       </c>
       <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>19</v>
       </c>
       <c r="B23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -1369,7 +1453,7 @@
         <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -1377,23 +1461,23 @@
         <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B36" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -1401,23 +1485,23 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -1425,14 +1509,30 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>4</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B46" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Clean up docs and reorganize images
- Remove old planning docs (ANDROID-SIGNING-SETUP, EVENT-SCREEN-REDESIGN, FLUTTER-PLAN, STARTUP-PROMPT)
- Move images to docs/Images/ folder
- Update DB-Schema and TEST-SCENARIOS
- Add App Store login notes

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/TEST-SCENARIOS.xlsx
+++ b/docs/TEST-SCENARIOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meetwithfriends\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA33429-A68F-43BF-BB40-CC6FD3DBAD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D943BFF-D1F0-4C9D-A615-7A7AF171A419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8C4B8439-3C7D-4BF3-9C30-18CFD3954126}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="52">
   <si>
     <t>Category</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Member changes RSVP to Not Going</t>
   </si>
   <si>
-    <t>Member cancels RSVP (back to no response)</t>
-  </si>
-  <si>
     <t>RSVP - Waitlist</t>
   </si>
   <si>
@@ -184,9 +181,6 @@
   </si>
   <si>
     <t>noodev8</t>
-  </si>
-  <si>
-    <t>Host assigns another host</t>
   </si>
 </sst>
 </file>
@@ -1054,11 +1048,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20932B91-48DE-46D3-9489-6C50CBF35969}">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1079,10 +1073,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -1095,13 +1089,13 @@
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="F2" s="3"/>
     </row>
@@ -1113,13 +1107,13 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1130,13 +1124,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1144,16 +1138,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1164,13 +1158,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1181,13 +1175,13 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1198,13 +1192,13 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1212,16 +1206,16 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1232,13 +1226,13 @@
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1249,13 +1243,13 @@
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1266,13 +1260,13 @@
         <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1283,13 +1277,13 @@
         <v>14</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1300,13 +1294,13 @@
         <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1317,13 +1311,13 @@
         <v>16</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1334,13 +1328,13 @@
         <v>17</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1351,13 +1345,13 @@
         <v>18</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1367,6 +1361,15 @@
       <c r="B20" t="s">
         <v>20</v>
       </c>
+      <c r="C20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -1375,6 +1378,15 @@
       <c r="B21" t="s">
         <v>21</v>
       </c>
+      <c r="C21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -1391,6 +1403,15 @@
       <c r="B23" t="s">
         <v>23</v>
       </c>
+      <c r="C23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -1399,13 +1420,31 @@
       <c r="B24" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" t="s">
-        <v>53</v>
+      <c r="C24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1413,127 +1452,120 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" t="s">
         <v>27</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>36</v>
-      </c>
-      <c r="B39" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>40</v>
-      </c>
-      <c r="B43" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="B44" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>4</v>
-      </c>
-      <c r="B46" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>